<commit_message>
(JMT) Added coverage to bl_1s14
</commit_message>
<xml_diff>
--- a/blocks/bl_1s14/bl_1s14.xlsx
+++ b/blocks/bl_1s14/bl_1s14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Foretellix\Files\workspace\AV_ValidationVerification\blocks\bl_1s14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D804201E-FE49-4B8E-B702-5B694F2590C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B29D3C6-13E2-4DAA-B80C-4A2A46663A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>runs</t>
   </si>
@@ -64,9 +64,6 @@
     <t>[-10..10]m</t>
   </si>
   <si>
-    <t>[-5..5]m</t>
-  </si>
-  <si>
     <t>npc_increase_speed</t>
   </si>
   <si>
@@ -83,6 +80,12 @@
   </si>
   <si>
     <t>[0..10]kph</t>
+  </si>
+  <si>
+    <t>[-10..10]kph</t>
+  </si>
+  <si>
+    <t>[-5..15]m</t>
   </si>
 </sst>
 </file>
@@ -926,7 +929,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,10 +949,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -969,7 +972,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -1004,22 +1007,22 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>